<commit_message>
fixing data format (removed unnecessary spaces)
</commit_message>
<xml_diff>
--- a/BioStats/FinalProject/finalProjData.xlsx
+++ b/BioStats/FinalProject/finalProjData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Windows\ServiceProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_1a90\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7C096021-9977-B843-83AD-3AAD28B4872F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{7C096021-9977-B843-83AD-3AAD28B4872F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0268E3BD-1E19-ED4F-B6C9-1B78A235A158}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="932" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="932" uniqueCount="36">
   <si>
     <t>CO</t>
   </si>
@@ -100,9 +100,6 @@
     <t>Fertilizer treatment</t>
   </si>
   <si>
-    <t>Fertilizer Treatment</t>
-  </si>
-  <si>
     <t>total biomass (g m-2 ) sampled at  the peak of standing biomass in mid-summer from 12 randomly selected 25cm x 25 cm grid cells from 144 cells per plot</t>
   </si>
   <si>
@@ -119,6 +116,27 @@
   </si>
   <si>
     <t>all non-clonal species biomass (g m-2 ) contributing to the total sampled biomass</t>
+  </si>
+  <si>
+    <t>FertilizerTreatment</t>
+  </si>
+  <si>
+    <t>TotalSpp#</t>
+  </si>
+  <si>
+    <t>NCSpp#</t>
+  </si>
+  <si>
+    <t>ClonSpp#</t>
+  </si>
+  <si>
+    <t>TotalBMS</t>
+  </si>
+  <si>
+    <t>NCBMS</t>
+  </si>
+  <si>
+    <t>ClonBMS</t>
   </si>
 </sst>
 </file>
@@ -503,7 +521,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B30" sqref="B30"/>
     </sheetView>
@@ -560,7 +578,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
@@ -568,7 +586,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
@@ -576,7 +594,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
@@ -584,7 +602,7 @@
         <v>14</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
@@ -592,7 +610,7 @@
         <v>15</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
@@ -600,7 +618,7 @@
         <v>16</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -612,9 +630,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G321"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.75" x14ac:dyDescent="0.15"/>
@@ -640,16 +658,16 @@
         <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
@@ -8024,7 +8042,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.75" x14ac:dyDescent="0.15"/>
@@ -8048,16 +8066,16 @@
         <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">

</xml_diff>